<commit_message>
Updating forms 3FA, adding forms 3DA
</commit_message>
<xml_diff>
--- a/forms/Form-3FA-multiple.xlsx
+++ b/forms/Form-3FA-multiple.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git\bitbucket_workspaces\IOTC-ws\R libs\workflow\forms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\dev\git\BitBucket workspaces\IOTC-ws\R libs\workflow\forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A949E724-177E-4C9A-90B2-DD57D056658E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC5656A-A14A-471A-AC4E-61C149DF2384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="XIpU8TyyplAxt8QCmvUzJLzka5iPLg/Syn8lyzD7JnF14tHCWyDvwRUY8XkQvaUmDTF8QPqODQN8PW7VsRXUGA==" workbookSaltValue="5qal3ZsWJINY7ZPEJSDbng==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{742ED9EC-8AD9-42B2-9B99-191B35B67816}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{742ED9EC-8AD9-42B2-9B99-191B35B67816}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -5355,7 +5355,7 @@
       <c r="BO55" s="22"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="AnC6/meggyljWeoXdmIh3mGtpbQOuSFehO83H3QY/hxk6PNfP062qY0jPJzjTsH5Ue3qQD3WC/4xdq/dD2wr0Q==" saltValue="0K+2Jzw4zqHxRbFRCQz+VQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Z0W20M7jgXESlWCQy1/aPtg/fPg8ERNerXhUNH6y5Nn0Rcr8FhBI7q0wnWQ49Ko+SqS2o55ccZy6cZiVx/5z5w==" saltValue="7zCJ7LKFDmZl4psxl/2hgA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="7">
     <mergeCell ref="R4:BO4"/>
     <mergeCell ref="B2:BO3"/>

</xml_diff>